<commit_message>
AutoCommit_11 сентября 2023 г. 10:26:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>ок</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                                                                                                           </t>
   </si>
 </sst>
 </file>
@@ -506,10 +509,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -664,7 +667,9 @@
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
@@ -675,7 +680,9 @@
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
@@ -721,7 +728,9 @@
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
@@ -732,7 +741,9 @@
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 сентября 2023 г. 11:27:29_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -512,7 +512,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12:C14"/>
+      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -599,7 +599,9 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
@@ -894,7 +896,9 @@
       <c r="B33" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_11 сентября 2023 г. 12:40:42_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -512,7 +512,7 @@
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -647,7 +647,9 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_19 сентября 2023 г. 11:26:28_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
+++ b/2ИСИП-122_Дискретная математика с элементами математической логики_I семестр.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>2ИСИП-122: Дискретная математика с элементами математической логики (Сибирев И. В.) - I семестр</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                                                                                                                                           </t>
+  </si>
+  <si>
+    <t>Дз2</t>
   </si>
 </sst>
 </file>
@@ -509,10 +512,10 @@
   <dimension ref="A1:W35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="4" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -551,7 +554,9 @@
       <c r="C3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:23" ht="13" x14ac:dyDescent="0.25">
@@ -650,7 +655,9 @@
       <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:23" ht="13" x14ac:dyDescent="0.25">
@@ -833,7 +840,9 @@
       <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" ht="13" x14ac:dyDescent="0.25">

</xml_diff>